<commit_message>
update db + m script
</commit_message>
<xml_diff>
--- a/Database/Campean/Frontiera.xlsx
+++ b/Database/Campean/Frontiera.xlsx
@@ -1,25 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23223"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\horva\Desktop\Practica\Practica_covid19_UTCN\Database\Campean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A5F94B-E42C-4AC6-968D-923CDE3CE55F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A929F379-EB90-44D3-B669-23B85348D2C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="380" windowWidth="24840" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -28,15 +31,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="8">
-  <si>
-    <t>diferenta</t>
-  </si>
-  <si>
-    <t>cazuri_covid</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
   <si>
     <t>data</t>
   </si>
@@ -52,12 +46,21 @@
   <si>
     <t>Auto frontiera</t>
   </si>
+  <si>
+    <t>diferenta</t>
+  </si>
+  <si>
+    <t>cazuri_covid</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -404,56 +407,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J216"/>
+  <dimension ref="A1:J224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
-      <selection activeCell="B209" sqref="B209:B216"/>
+    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
+      <selection activeCell="K226" sqref="K226"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" customWidth="1"/>
-    <col min="4" max="4" width="11.1796875" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="13.81640625" customWidth="1"/>
-    <col min="7" max="7" width="11.81640625" customWidth="1"/>
-    <col min="8" max="8" width="13.81640625" customWidth="1"/>
-    <col min="9" max="9" width="13.08984375" customWidth="1"/>
-    <col min="10" max="10" width="12.453125" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>43838</v>
       </c>
@@ -482,7 +485,7 @@
         <v>-30500</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>43839</v>
       </c>
@@ -511,7 +514,7 @@
         <v>-17200</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>43840</v>
       </c>
@@ -540,7 +543,7 @@
         <v>-26400</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>43843</v>
       </c>
@@ -569,7 +572,7 @@
         <v>-31200</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>43844</v>
       </c>
@@ -598,7 +601,7 @@
         <v>-9500</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>43845</v>
       </c>
@@ -627,7 +630,7 @@
         <v>-17000</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>43846</v>
       </c>
@@ -656,7 +659,7 @@
         <v>-8600</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>43847</v>
       </c>
@@ -685,7 +688,7 @@
         <v>-19100</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>43850</v>
       </c>
@@ -714,7 +717,7 @@
         <v>-6800</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>43851</v>
       </c>
@@ -743,7 +746,7 @@
         <v>-6700</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>43852</v>
       </c>
@@ -772,7 +775,7 @@
         <v>-11300</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>43853</v>
       </c>
@@ -801,7 +804,7 @@
         <v>-10200</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>43854</v>
       </c>
@@ -830,7 +833,7 @@
         <v>-24700</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>43855</v>
       </c>
@@ -859,7 +862,7 @@
         <v>-23800</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>43856</v>
       </c>
@@ -888,7 +891,7 @@
         <v>-2400</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9">
       <c r="A17" s="1">
         <v>43858</v>
       </c>
@@ -917,7 +920,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9">
       <c r="A18" s="1">
         <v>43859</v>
       </c>
@@ -946,7 +949,7 @@
         <v>-4300</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9">
       <c r="A19" s="1">
         <v>43860</v>
       </c>
@@ -975,7 +978,7 @@
         <v>-7300</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9">
       <c r="A20" s="1">
         <v>43861</v>
       </c>
@@ -1004,7 +1007,7 @@
         <v>-7400</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9">
       <c r="A21" s="1">
         <v>43862</v>
       </c>
@@ -1012,28 +1015,28 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D21" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F21" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G21" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H21" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I21" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" s="1">
         <v>43863</v>
       </c>
@@ -1041,28 +1044,28 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D22" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F22" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G22" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H22" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I22" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="1">
         <v>43864</v>
       </c>
@@ -1091,7 +1094,7 @@
         <v>-2500</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9">
       <c r="A24" s="1">
         <v>43865</v>
       </c>
@@ -1120,7 +1123,7 @@
         <v>-3800</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9">
       <c r="A25" s="1">
         <v>43866</v>
       </c>
@@ -1149,7 +1152,7 @@
         <v>-5100</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9">
       <c r="A26" s="1">
         <v>43867</v>
       </c>
@@ -1178,7 +1181,7 @@
         <v>-3600</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9">
       <c r="A27" s="1">
         <v>43868</v>
       </c>
@@ -1207,7 +1210,7 @@
         <v>-8100</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9">
       <c r="A28" s="1">
         <v>43869</v>
       </c>
@@ -1236,7 +1239,7 @@
         <v>-14000</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9">
       <c r="A29" s="1">
         <v>43871</v>
       </c>
@@ -1265,7 +1268,7 @@
         <v>-2800</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9">
       <c r="A30" s="1">
         <v>43872</v>
       </c>
@@ -1294,7 +1297,7 @@
         <v>-5900</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9">
       <c r="A31" s="1">
         <v>43873</v>
       </c>
@@ -1323,7 +1326,7 @@
         <v>-8100</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9">
       <c r="A32" s="1">
         <v>43874</v>
       </c>
@@ -1352,7 +1355,7 @@
         <v>-1800</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10">
       <c r="A33" s="1">
         <v>43875</v>
       </c>
@@ -1381,7 +1384,7 @@
         <v>-6200</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10">
       <c r="A34" s="1">
         <v>43878</v>
       </c>
@@ -1410,7 +1413,7 @@
         <v>-4800</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10">
       <c r="A35" s="1">
         <v>43879</v>
       </c>
@@ -1439,7 +1442,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10">
       <c r="A36" s="1">
         <v>43880</v>
       </c>
@@ -1468,7 +1471,7 @@
         <v>-4900</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10">
       <c r="A37" s="1">
         <v>43881</v>
       </c>
@@ -1497,7 +1500,7 @@
         <v>-3400</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10">
       <c r="A38" s="1">
         <v>43883</v>
       </c>
@@ -1526,7 +1529,7 @@
         <v>-6400</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10">
       <c r="A39" s="1">
         <v>43884</v>
       </c>
@@ -1555,7 +1558,7 @@
         <v>-2600</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10">
       <c r="A40" s="1">
         <v>43885</v>
       </c>
@@ -1584,7 +1587,7 @@
         <v>-1600</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10">
       <c r="A41" s="1">
         <v>43886</v>
       </c>
@@ -1613,7 +1616,7 @@
         <v>4400</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10">
       <c r="A42" s="1">
         <v>43887</v>
       </c>
@@ -1645,7 +1648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10">
       <c r="A43" s="1">
         <v>43888</v>
       </c>
@@ -1677,7 +1680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10">
       <c r="A44" s="1">
         <v>43889</v>
       </c>
@@ -1709,7 +1712,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10">
       <c r="A45" s="1">
         <v>43890</v>
       </c>
@@ -1741,7 +1744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10">
       <c r="A46" s="1">
         <v>43891</v>
       </c>
@@ -1773,7 +1776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10">
       <c r="A47" s="1">
         <v>43892</v>
       </c>
@@ -1805,7 +1808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10">
       <c r="A48" s="1">
         <v>43893</v>
       </c>
@@ -1837,7 +1840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10">
       <c r="A49" s="1">
         <v>43894</v>
       </c>
@@ -1869,7 +1872,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10">
       <c r="A50" s="1">
         <v>43895</v>
       </c>
@@ -1901,7 +1904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10">
       <c r="A51" s="1">
         <v>43896</v>
       </c>
@@ -1933,7 +1936,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10">
       <c r="A52" s="1">
         <v>43897</v>
       </c>
@@ -1965,7 +1968,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10">
       <c r="A53" s="1">
         <v>43898</v>
       </c>
@@ -1997,7 +2000,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10">
       <c r="A54" s="1">
         <v>43899</v>
       </c>
@@ -2029,7 +2032,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10">
       <c r="A55" s="1">
         <v>43900</v>
       </c>
@@ -2061,7 +2064,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10">
       <c r="A56" s="1">
         <v>43901</v>
       </c>
@@ -2093,7 +2096,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10">
       <c r="A57" s="1">
         <v>43902</v>
       </c>
@@ -2125,7 +2128,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10">
       <c r="A58" s="1">
         <v>43903</v>
       </c>
@@ -2157,7 +2160,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10">
       <c r="A59" s="1">
         <v>43904</v>
       </c>
@@ -2189,7 +2192,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10">
       <c r="A60" s="1">
         <v>43905</v>
       </c>
@@ -2221,7 +2224,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10">
       <c r="A61" s="1">
         <v>43906</v>
       </c>
@@ -2253,7 +2256,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10">
       <c r="A62" s="1">
         <v>43907</v>
       </c>
@@ -2285,7 +2288,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10">
       <c r="A63" s="1">
         <v>43908</v>
       </c>
@@ -2317,7 +2320,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10">
       <c r="A64" s="1">
         <v>43909</v>
       </c>
@@ -2349,7 +2352,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10">
       <c r="A65" s="1">
         <v>43910</v>
       </c>
@@ -2381,7 +2384,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10">
       <c r="A66" s="1">
         <v>43911</v>
       </c>
@@ -2413,7 +2416,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10">
       <c r="A67" s="1">
         <v>43912</v>
       </c>
@@ -2445,7 +2448,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10">
       <c r="A68" s="1">
         <v>43913</v>
       </c>
@@ -2477,7 +2480,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10">
       <c r="A69" s="1">
         <v>43914</v>
       </c>
@@ -2509,7 +2512,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10">
       <c r="A70" s="1">
         <v>43915</v>
       </c>
@@ -2541,7 +2544,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10">
       <c r="A71" s="1">
         <v>43916</v>
       </c>
@@ -2573,7 +2576,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10">
       <c r="A72" s="1">
         <v>43917</v>
       </c>
@@ -2605,7 +2608,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10">
       <c r="A73" s="1">
         <v>43918</v>
       </c>
@@ -2637,7 +2640,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10">
       <c r="A74" s="1">
         <v>43919</v>
       </c>
@@ -2669,7 +2672,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10">
       <c r="A75" s="1">
         <v>43920</v>
       </c>
@@ -2701,7 +2704,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10">
       <c r="A76" s="1">
         <v>43921</v>
       </c>
@@ -2733,7 +2736,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10">
       <c r="A77" s="1">
         <v>43922</v>
       </c>
@@ -2765,7 +2768,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10">
       <c r="A78" s="1">
         <v>43923</v>
       </c>
@@ -2797,7 +2800,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10">
       <c r="A79" s="1">
         <v>43924</v>
       </c>
@@ -2829,7 +2832,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10">
       <c r="A80" s="1">
         <v>43925</v>
       </c>
@@ -2861,7 +2864,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10">
       <c r="A81" s="1">
         <v>43926</v>
       </c>
@@ -2893,7 +2896,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10">
       <c r="A82" s="1">
         <v>43927</v>
       </c>
@@ -2925,7 +2928,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10">
       <c r="A83" s="1">
         <v>43928</v>
       </c>
@@ -2957,7 +2960,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10">
       <c r="A84" s="1">
         <v>43929</v>
       </c>
@@ -2989,7 +2992,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10">
       <c r="A85" s="1">
         <v>43930</v>
       </c>
@@ -3021,7 +3024,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10">
       <c r="A86" s="1">
         <v>43931</v>
       </c>
@@ -3053,7 +3056,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10">
       <c r="A87" s="1">
         <v>43932</v>
       </c>
@@ -3085,7 +3088,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10">
       <c r="A88" s="1">
         <v>43933</v>
       </c>
@@ -3117,7 +3120,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10">
       <c r="A89" s="1">
         <v>43934</v>
       </c>
@@ -3149,7 +3152,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10">
       <c r="A90" s="1">
         <v>43935</v>
       </c>
@@ -3181,7 +3184,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10">
       <c r="A91" s="1">
         <v>43936</v>
       </c>
@@ -3213,7 +3216,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10">
       <c r="A92" s="1">
         <v>43937</v>
       </c>
@@ -3245,7 +3248,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10">
       <c r="A93" s="1">
         <v>43938</v>
       </c>
@@ -3277,7 +3280,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10">
       <c r="A94" s="1">
         <v>43939</v>
       </c>
@@ -3309,7 +3312,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10">
       <c r="A95" s="1">
         <v>43940</v>
       </c>
@@ -3341,7 +3344,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10">
       <c r="A96" s="1">
         <v>43941</v>
       </c>
@@ -3373,7 +3376,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10">
       <c r="A97" s="1">
         <v>43942</v>
       </c>
@@ -3405,7 +3408,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10">
       <c r="A98" s="1">
         <v>43943</v>
       </c>
@@ -3437,7 +3440,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10">
       <c r="A99" s="1">
         <v>43944</v>
       </c>
@@ -3469,7 +3472,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10">
       <c r="A100" s="1">
         <v>43945</v>
       </c>
@@ -3501,7 +3504,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10">
       <c r="A101" s="1">
         <v>43946</v>
       </c>
@@ -3533,7 +3536,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:10">
       <c r="A102" s="1">
         <v>43947</v>
       </c>
@@ -3565,7 +3568,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:10">
       <c r="A103" s="1">
         <v>43948</v>
       </c>
@@ -3597,7 +3600,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:10">
       <c r="A104" s="1">
         <v>43949</v>
       </c>
@@ -3629,7 +3632,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:10">
       <c r="A105" s="1">
         <v>43950</v>
       </c>
@@ -3661,7 +3664,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:10">
       <c r="A106" s="1">
         <v>43951</v>
       </c>
@@ -3693,7 +3696,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:10">
       <c r="A107" s="1">
         <v>43952</v>
       </c>
@@ -3725,7 +3728,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:10">
       <c r="A108" s="1">
         <v>43953</v>
       </c>
@@ -3757,7 +3760,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:10">
       <c r="A109" s="1">
         <v>43954</v>
       </c>
@@ -3789,7 +3792,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:10">
       <c r="A110" s="1">
         <v>43955</v>
       </c>
@@ -3821,7 +3824,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:10">
       <c r="A111" s="1">
         <v>43956</v>
       </c>
@@ -3853,7 +3856,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:10">
       <c r="A112" s="1">
         <v>43957</v>
       </c>
@@ -3885,7 +3888,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:10">
       <c r="A113" s="1">
         <v>43958</v>
       </c>
@@ -3917,7 +3920,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:10">
       <c r="A114" s="1">
         <v>43959</v>
       </c>
@@ -3949,7 +3952,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:10">
       <c r="A115" s="1">
         <v>43960</v>
       </c>
@@ -3981,7 +3984,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:10">
       <c r="A116" s="1">
         <v>43961</v>
       </c>
@@ -4013,7 +4016,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:10">
       <c r="A117" s="1">
         <v>43962</v>
       </c>
@@ -4045,7 +4048,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:10">
       <c r="A118" s="1">
         <v>43963</v>
       </c>
@@ -4077,7 +4080,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:10">
       <c r="A119" s="1">
         <v>43964</v>
       </c>
@@ -4109,7 +4112,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:10">
       <c r="A120" s="1">
         <v>43965</v>
       </c>
@@ -4141,7 +4144,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:10">
       <c r="A121" s="1">
         <v>43966</v>
       </c>
@@ -4173,7 +4176,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:10">
       <c r="A122" s="1">
         <v>43967</v>
       </c>
@@ -4205,7 +4208,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:10">
       <c r="A123" s="1">
         <v>43968</v>
       </c>
@@ -4237,7 +4240,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:10">
       <c r="A124" s="1">
         <v>43969</v>
       </c>
@@ -4269,7 +4272,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:10">
       <c r="A125" s="1">
         <v>43970</v>
       </c>
@@ -4301,7 +4304,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:10">
       <c r="A126" s="1">
         <v>43971</v>
       </c>
@@ -4333,7 +4336,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:10">
       <c r="A127" s="1">
         <v>43972</v>
       </c>
@@ -4365,7 +4368,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:10">
       <c r="A128" s="1">
         <v>43973</v>
       </c>
@@ -4397,7 +4400,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:10">
       <c r="A129" s="1">
         <v>43974</v>
       </c>
@@ -4429,7 +4432,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:10">
       <c r="A130" s="1">
         <v>43975</v>
       </c>
@@ -4461,7 +4464,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:10">
       <c r="A131" s="1">
         <v>43976</v>
       </c>
@@ -4493,7 +4496,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:10">
       <c r="A132" s="1">
         <v>43977</v>
       </c>
@@ -4525,7 +4528,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:10">
       <c r="A133" s="1">
         <v>43978</v>
       </c>
@@ -4557,7 +4560,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:10">
       <c r="A134" s="1">
         <v>43979</v>
       </c>
@@ -4589,7 +4592,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:10">
       <c r="A135" s="1">
         <v>43980</v>
       </c>
@@ -4621,7 +4624,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:10">
       <c r="A136" s="1">
         <v>43981</v>
       </c>
@@ -4629,31 +4632,31 @@
         <v>135</v>
       </c>
       <c r="C136" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D136" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E136" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F136" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G136" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H136" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I136" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="J136">
         <v>151</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:10">
       <c r="A137" s="1">
         <v>43982</v>
       </c>
@@ -4685,7 +4688,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:10">
       <c r="A138" s="1">
         <v>43983</v>
       </c>
@@ -4717,7 +4720,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:10">
       <c r="A139" s="1">
         <v>43984</v>
       </c>
@@ -4749,7 +4752,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:10">
       <c r="A140" s="1">
         <v>43985</v>
       </c>
@@ -4781,7 +4784,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:10">
       <c r="A141" s="1">
         <v>43986</v>
       </c>
@@ -4813,7 +4816,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:10">
       <c r="A142" s="1">
         <v>43987</v>
       </c>
@@ -4845,7 +4848,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:10">
       <c r="A143" s="1">
         <v>43988</v>
       </c>
@@ -4877,7 +4880,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:10">
       <c r="A144" s="1">
         <v>43989</v>
       </c>
@@ -4909,7 +4912,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:10">
       <c r="A145" s="1">
         <v>43990</v>
       </c>
@@ -4941,7 +4944,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:10">
       <c r="A146" s="1">
         <v>43991</v>
       </c>
@@ -4973,7 +4976,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:10">
       <c r="A147" s="1">
         <v>43992</v>
       </c>
@@ -5005,7 +5008,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:10">
       <c r="A148" s="1">
         <v>43993</v>
       </c>
@@ -5037,7 +5040,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:10">
       <c r="A149" s="1">
         <v>43994</v>
       </c>
@@ -5069,7 +5072,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:10">
       <c r="A150" s="1">
         <v>43995</v>
       </c>
@@ -5101,7 +5104,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:10">
       <c r="A151" s="1">
         <v>43996</v>
       </c>
@@ -5133,7 +5136,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:10">
       <c r="A152" s="1">
         <v>43997</v>
       </c>
@@ -5165,7 +5168,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:10">
       <c r="A153" s="1">
         <v>43998</v>
       </c>
@@ -5197,7 +5200,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:10">
       <c r="A154" s="1">
         <v>43999</v>
       </c>
@@ -5229,7 +5232,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:10">
       <c r="A155" s="1">
         <v>44000</v>
       </c>
@@ -5261,7 +5264,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:10">
       <c r="A156" s="1">
         <v>44001</v>
       </c>
@@ -5293,7 +5296,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:10">
       <c r="A157" s="1">
         <v>44002</v>
       </c>
@@ -5325,7 +5328,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:10">
       <c r="A158" s="1">
         <v>44003</v>
       </c>
@@ -5357,7 +5360,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:10">
       <c r="A159" s="1">
         <v>44004</v>
       </c>
@@ -5389,7 +5392,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:10">
       <c r="A160" s="1">
         <v>44005</v>
       </c>
@@ -5421,7 +5424,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:10">
       <c r="A161" s="1">
         <v>44006</v>
       </c>
@@ -5453,7 +5456,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:10">
       <c r="A162" s="1">
         <v>44007</v>
       </c>
@@ -5485,7 +5488,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:10">
       <c r="A163" s="1">
         <v>44008</v>
       </c>
@@ -5517,7 +5520,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:10">
       <c r="A164" s="1">
         <v>44009</v>
       </c>
@@ -5549,7 +5552,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:10">
       <c r="A165" s="1">
         <v>44010</v>
       </c>
@@ -5581,7 +5584,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:10">
       <c r="A166" s="1">
         <v>44011</v>
       </c>
@@ -5613,7 +5616,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:10">
       <c r="A167" s="1">
         <v>44012</v>
       </c>
@@ -5645,7 +5648,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:10">
       <c r="A168" s="1">
         <v>44013</v>
       </c>
@@ -5677,7 +5680,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:10">
       <c r="A169" s="1">
         <v>44014</v>
       </c>
@@ -5709,7 +5712,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:10">
       <c r="A170" s="1">
         <v>44015</v>
       </c>
@@ -5741,7 +5744,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:10">
       <c r="A171" s="1">
         <v>44016</v>
       </c>
@@ -5773,7 +5776,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:10">
       <c r="A172" s="1">
         <v>44017</v>
       </c>
@@ -5805,7 +5808,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:10">
       <c r="A173" s="1">
         <v>44018</v>
       </c>
@@ -5837,7 +5840,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:10">
       <c r="A174" s="1">
         <v>44019</v>
       </c>
@@ -5869,7 +5872,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:10">
       <c r="A175" s="1">
         <v>44020</v>
       </c>
@@ -5901,7 +5904,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:10">
       <c r="A176" s="1">
         <v>44021</v>
       </c>
@@ -5933,7 +5936,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:10">
       <c r="A177" s="1">
         <v>44022</v>
       </c>
@@ -5965,7 +5968,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:10">
       <c r="A178" s="1">
         <v>44023</v>
       </c>
@@ -5997,7 +6000,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:10">
       <c r="A179" s="1">
         <v>44024</v>
       </c>
@@ -6029,7 +6032,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:10">
       <c r="A180" s="1">
         <v>44025</v>
       </c>
@@ -6061,7 +6064,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:10">
       <c r="A181" s="1">
         <v>44026</v>
       </c>
@@ -6093,7 +6096,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:10">
       <c r="A182" s="1">
         <v>44027</v>
       </c>
@@ -6125,7 +6128,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:10">
       <c r="A183" s="1">
         <v>44028</v>
       </c>
@@ -6157,7 +6160,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:10">
       <c r="A184" s="1">
         <v>44029</v>
       </c>
@@ -6189,7 +6192,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:10">
       <c r="A185" s="1">
         <v>44030</v>
       </c>
@@ -6221,7 +6224,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:10">
       <c r="A186" s="1">
         <v>44031</v>
       </c>
@@ -6253,7 +6256,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:10">
       <c r="A187" s="1">
         <v>44032</v>
       </c>
@@ -6285,7 +6288,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:10">
       <c r="A188" s="1">
         <v>44033</v>
       </c>
@@ -6317,7 +6320,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:10">
       <c r="A189" s="1">
         <v>44034</v>
       </c>
@@ -6349,7 +6352,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:10">
       <c r="A190" s="1">
         <v>44035</v>
       </c>
@@ -6381,7 +6384,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:10">
       <c r="A191" s="1">
         <v>44036</v>
       </c>
@@ -6413,7 +6416,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:10">
       <c r="A192" s="1">
         <v>44037</v>
       </c>
@@ -6445,7 +6448,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:9">
       <c r="A193" s="1">
         <v>44038</v>
       </c>
@@ -6474,7 +6477,7 @@
         <v>8100</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:9">
       <c r="A194" s="1">
         <v>44039</v>
       </c>
@@ -6503,7 +6506,7 @@
         <v>4300</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:9">
       <c r="A195" s="1">
         <v>44040</v>
       </c>
@@ -6532,7 +6535,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:9">
       <c r="A196" s="1">
         <v>44041</v>
       </c>
@@ -6561,7 +6564,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:9">
       <c r="A197" s="1">
         <v>44042</v>
       </c>
@@ -6590,7 +6593,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:9">
       <c r="A198" s="1">
         <v>44043</v>
       </c>
@@ -6619,7 +6622,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:9">
       <c r="A199" s="1">
         <v>44044</v>
       </c>
@@ -6648,7 +6651,7 @@
         <v>15700</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:9">
       <c r="A200" s="1">
         <v>44045</v>
       </c>
@@ -6677,7 +6680,7 @@
         <v>13800</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:9">
       <c r="A201" s="1">
         <v>44046</v>
       </c>
@@ -6706,7 +6709,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:9">
       <c r="A202" s="1">
         <v>44047</v>
       </c>
@@ -6735,7 +6738,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:9">
       <c r="A203" s="1">
         <v>44048</v>
       </c>
@@ -6764,7 +6767,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:9">
       <c r="A204" s="1">
         <v>44049</v>
       </c>
@@ -6793,7 +6796,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:9">
       <c r="A205" s="1">
         <v>44050</v>
       </c>
@@ -6822,7 +6825,7 @@
         <v>-400</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:9">
       <c r="A206" s="1">
         <v>44051</v>
       </c>
@@ -6851,7 +6854,7 @@
         <v>6400</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:9">
       <c r="A207" s="1">
         <v>44052</v>
       </c>
@@ -6880,7 +6883,7 @@
         <v>10300</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:9">
       <c r="A208" s="1">
         <v>44053</v>
       </c>
@@ -6909,7 +6912,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:9">
       <c r="A209" s="1">
         <v>44054</v>
       </c>
@@ -6938,7 +6941,7 @@
         <v>-1900</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:9">
       <c r="A210" s="1">
         <v>44055</v>
       </c>
@@ -6967,7 +6970,7 @@
         <v>-1000</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:9">
       <c r="A211" s="1">
         <v>44056</v>
       </c>
@@ -6996,7 +6999,7 @@
         <v>-5100</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:9">
       <c r="A212" s="1">
         <v>44057</v>
       </c>
@@ -7025,7 +7028,7 @@
         <v>-5300</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:9">
       <c r="A213" s="1">
         <v>44058</v>
       </c>
@@ -7054,7 +7057,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:9">
       <c r="A214" s="1">
         <v>44059</v>
       </c>
@@ -7083,7 +7086,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:9">
       <c r="A215" s="1">
         <v>44060</v>
       </c>
@@ -7112,7 +7115,7 @@
         <v>-5600</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:9">
       <c r="A216" s="1">
         <v>44061</v>
       </c>
@@ -7139,6 +7142,238 @@
       </c>
       <c r="I216">
         <v>-4200</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9">
+      <c r="A217" s="1">
+        <v>44062</v>
+      </c>
+      <c r="B217" s="2">
+        <v>216</v>
+      </c>
+      <c r="C217">
+        <v>82600</v>
+      </c>
+      <c r="D217">
+        <v>39300</v>
+      </c>
+      <c r="E217">
+        <v>43300</v>
+      </c>
+      <c r="F217">
+        <v>30900</v>
+      </c>
+      <c r="G217">
+        <v>14500</v>
+      </c>
+      <c r="H217">
+        <v>16400</v>
+      </c>
+      <c r="I217">
+        <v>-4000</v>
+      </c>
+    </row>
+    <row r="218" spans="1:9">
+      <c r="A218" s="1">
+        <v>44063</v>
+      </c>
+      <c r="B218" s="2">
+        <v>217</v>
+      </c>
+      <c r="C218">
+        <v>80900</v>
+      </c>
+      <c r="D218">
+        <v>37000</v>
+      </c>
+      <c r="E218">
+        <v>43900</v>
+      </c>
+      <c r="F218">
+        <v>25600</v>
+      </c>
+      <c r="G218">
+        <v>12100</v>
+      </c>
+      <c r="H218">
+        <v>13500</v>
+      </c>
+      <c r="I218">
+        <v>-6900</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9">
+      <c r="A219" s="1">
+        <v>44064</v>
+      </c>
+      <c r="B219" s="2">
+        <v>218</v>
+      </c>
+      <c r="C219">
+        <v>98300</v>
+      </c>
+      <c r="D219">
+        <v>44900</v>
+      </c>
+      <c r="E219">
+        <v>53400</v>
+      </c>
+      <c r="F219">
+        <v>32600</v>
+      </c>
+      <c r="G219">
+        <v>16000</v>
+      </c>
+      <c r="H219">
+        <v>16600</v>
+      </c>
+      <c r="I219">
+        <v>-8500</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9">
+      <c r="A220" s="1">
+        <v>44065</v>
+      </c>
+      <c r="B220" s="2">
+        <v>219</v>
+      </c>
+      <c r="C220">
+        <v>101400</v>
+      </c>
+      <c r="D220">
+        <v>48300</v>
+      </c>
+      <c r="E220">
+        <v>53100</v>
+      </c>
+      <c r="F220">
+        <v>31900</v>
+      </c>
+      <c r="G220">
+        <v>16300</v>
+      </c>
+      <c r="H220">
+        <v>15600</v>
+      </c>
+      <c r="I220">
+        <v>-4800</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9">
+      <c r="A221" s="1">
+        <v>44066</v>
+      </c>
+      <c r="B221" s="2">
+        <v>220</v>
+      </c>
+      <c r="C221">
+        <v>95700</v>
+      </c>
+      <c r="D221">
+        <v>44300</v>
+      </c>
+      <c r="E221">
+        <v>51400</v>
+      </c>
+      <c r="F221">
+        <v>28100</v>
+      </c>
+      <c r="G221">
+        <v>13000</v>
+      </c>
+      <c r="H221">
+        <v>15100</v>
+      </c>
+      <c r="I221">
+        <v>-7100</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9">
+      <c r="A222" s="1">
+        <v>44067</v>
+      </c>
+      <c r="B222" s="2">
+        <v>221</v>
+      </c>
+      <c r="C222">
+        <v>86500</v>
+      </c>
+      <c r="D222">
+        <v>38200</v>
+      </c>
+      <c r="E222">
+        <v>48300</v>
+      </c>
+      <c r="F222">
+        <v>29700</v>
+      </c>
+      <c r="G222">
+        <v>13400</v>
+      </c>
+      <c r="H222">
+        <v>16300</v>
+      </c>
+      <c r="I222">
+        <v>-10100</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9">
+      <c r="A223" s="1">
+        <v>44068</v>
+      </c>
+      <c r="B223" s="2">
+        <v>222</v>
+      </c>
+      <c r="C223">
+        <v>81400</v>
+      </c>
+      <c r="D223">
+        <v>36700</v>
+      </c>
+      <c r="E223">
+        <v>44700</v>
+      </c>
+      <c r="F223">
+        <v>31000</v>
+      </c>
+      <c r="G223">
+        <v>14700</v>
+      </c>
+      <c r="H223">
+        <v>16300</v>
+      </c>
+      <c r="I223">
+        <v>-8000</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9">
+      <c r="A224" s="1">
+        <v>44069</v>
+      </c>
+      <c r="B224" s="2">
+        <v>223</v>
+      </c>
+      <c r="C224">
+        <v>83300</v>
+      </c>
+      <c r="D224">
+        <v>38300</v>
+      </c>
+      <c r="E224">
+        <v>45000</v>
+      </c>
+      <c r="F224">
+        <v>31000</v>
+      </c>
+      <c r="G224">
+        <v>15000</v>
+      </c>
+      <c r="H224">
+        <v>16000</v>
+      </c>
+      <c r="I224">
+        <v>-6700</v>
       </c>
     </row>
   </sheetData>

</xml_diff>